<commit_message>
full program whithout adding new lines to eq_base
</commit_message>
<xml_diff>
--- a/IP_calculation_Pro/equipment_database.xlsx
+++ b/IP_calculation_Pro/equipment_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\PycharmProjects\first_public_project\IP_calculation_Pro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C874CE-BECD-4CBE-82C6-1BD7C33B74CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A6BC47-38E6-483B-9AE3-7BCA8A91E8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
   <si>
     <t>equipment_name</t>
   </si>
@@ -145,6 +145,9 @@
     <t>10.5.31.255</t>
   </si>
   <si>
+    <t>close</t>
+  </si>
+  <si>
     <t>без мышей</t>
   </si>
   <si>
@@ -160,13 +163,16 @@
     <t>10.8.23.255</t>
   </si>
   <si>
-    <t>close</t>
-  </si>
-  <si>
     <t>10.7.22.1</t>
   </si>
   <si>
     <t>10.7.22.255</t>
+  </si>
+  <si>
+    <t>23.5.11.1</t>
+  </si>
+  <si>
+    <t>23.5.11.255</t>
   </si>
 </sst>
 </file>
@@ -529,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,7 +833,7 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -847,10 +853,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -859,21 +865,21 @@
         <v>255</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15">
         <v>256</v>
@@ -888,6 +894,52 @@
         <v>48</v>
       </c>
       <c r="G15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16">
+        <v>512</v>
+      </c>
+      <c r="D16">
+        <v>766</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17">
+        <v>512</v>
+      </c>
+      <c r="D17">
+        <v>766</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some new files with AI
</commit_message>
<xml_diff>
--- a/IP_calculation_Pro/equipment_database.xlsx
+++ b/IP_calculation_Pro/equipment_database.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\PycharmProjects\first_public_project\IP_calculation_Pro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A6BC47-38E6-483B-9AE3-7BCA8A91E8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC37B68-3884-48B9-BDC2-0F394D2ACD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>equipment_name</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>23.5.11.255</t>
+  </si>
+  <si>
+    <t>10.5.11.1</t>
+  </si>
+  <si>
+    <t>10.5.11.255</t>
   </si>
 </sst>
 </file>
@@ -535,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,7 +799,8 @@
         <v>5120</v>
       </c>
       <c r="D11">
-        <v>7659</v>
+        <f>C11+2558</f>
+        <v>7678</v>
       </c>
       <c r="E11" t="s">
         <v>35</v>
@@ -940,6 +947,31 @@
         <v>50</v>
       </c>
       <c r="G17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18">
+        <f>D15+1</f>
+        <v>511</v>
+      </c>
+      <c r="D18">
+        <f>C18+254</f>
+        <v>765</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>